<commit_message>
multiple requests/responses per TestCase, added metadata and exception for CoreService and Java
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4714539E-BC71-3046-9316-7D37F4CC2D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFD4A9C-199F-8F4D-BD0A-F3DE1AB7E518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="500" windowWidth="24420" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
   <si>
     <t>List of all config items</t>
   </si>
@@ -53,17 +55,434 @@
     <t>NOTE: All config should be managed by CoreService. Additionally, may refactor constants in test files to configs</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>Name (full config name)</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Name (Config property)</t>
+  </si>
+  <si>
+    <t>NodeJS deploy.js property</t>
+  </si>
+  <si>
+    <t>Java application.properties property</t>
+  </si>
+  <si>
+    <t>core.log.dir</t>
+  </si>
+  <si>
+    <t>logDir</t>
+  </si>
+  <si>
+    <t>Log directory for CoreService</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>./log</t>
+  </si>
+  <si>
+    <t>core.proto.descriptor.path</t>
+  </si>
+  <si>
+    <t>protoDescriptorPath</t>
+  </si>
+  <si>
+    <t>Path to .protobin file</t>
+  </si>
+  <si>
+    <t>protobin/common.protobin</t>
+  </si>
+  <si>
+    <t>core.custom-tests.classpath</t>
+  </si>
+  <si>
+    <t>customTestsClasspath</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>core.proto.classpath</t>
+  </si>
+  <si>
+    <t>protoClasspath</t>
+  </si>
+  <si>
+    <t>Classpath to directory containing .proto files</t>
+  </si>
+  <si>
+    <t>proto</t>
+  </si>
+  <si>
+    <t>Classpath to directory containing test cases (CoreService will translate these test cases to .bin files in test-cases/)</t>
+  </si>
+  <si>
+    <t>testsDir</t>
+  </si>
+  <si>
+    <t>Directory containing .bin test cases</t>
+  </si>
+  <si>
+    <t>core.out.tests.dir</t>
+  </si>
+  <si>
+    <t>test-cases</t>
+  </si>
+  <si>
+    <t>core.dev.debug.enabled</t>
+  </si>
+  <si>
+    <t>debugEnabled</t>
+  </si>
+  <si>
+    <t>Toggle debug mode (NOT IMPLEMENTED)</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>config.protoDir</t>
+  </si>
+  <si>
+    <t>proto/</t>
+  </si>
+  <si>
+    <t>config.log.dir</t>
+  </si>
+  <si>
+    <t>config.log.filename</t>
+  </si>
+  <si>
+    <t>log/</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.log.dir</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.log.file</t>
+  </si>
+  <si>
+    <t>nodejsClientLogDir</t>
+  </si>
+  <si>
+    <t>nodejsClientLogFile</t>
+  </si>
+  <si>
+    <t>Log file for NodeJs client</t>
+  </si>
+  <si>
+    <t>node-client.log</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.tests.dir</t>
+  </si>
+  <si>
+    <t>nodejsClientTestsDir</t>
+  </si>
+  <si>
+    <t>config.testcaseDir</t>
+  </si>
+  <si>
+    <t>test-cases/</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.out.dir</t>
+  </si>
+  <si>
+    <t>nodejsClientOutDir</t>
+  </si>
+  <si>
+    <t>Output directory for NodeJs client</t>
+  </si>
+  <si>
+    <t>NOTE: All configs related to client/server of a language is defined in context of the container running that client/server)</t>
+  </si>
+  <si>
+    <t>Log directory for NodeJs client</t>
+  </si>
+  <si>
+    <t>config.outDir</t>
+  </si>
+  <si>
+    <t>out/client/</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.server.host</t>
+  </si>
+  <si>
+    <t>nodejsClientServerHost</t>
+  </si>
+  <si>
+    <t>Hostname of the server to which NodeJs client connects to</t>
+  </si>
+  <si>
+    <t>config.server.host</t>
+  </si>
+  <si>
+    <t>APPENDIX A: LIST OF CONSTANTS</t>
+  </si>
+  <si>
+    <t>SERVER HOSTNAME</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.server.port</t>
+  </si>
+  <si>
+    <t>nodejsClientServerPort</t>
+  </si>
+  <si>
+    <t>Port of the server to which NodeJs client connects to</t>
+  </si>
+  <si>
+    <t>config.server.port</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>java-server</t>
+  </si>
+  <si>
+    <t>node-server</t>
+  </si>
+  <si>
+    <t>test.nodejs.client.proto.dir</t>
+  </si>
+  <si>
+    <t>nodejsClientProtoDir</t>
+  </si>
+  <si>
+    <t>Directory containing .proto files for nodejs client</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.proto.dir</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.log.dir</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.log.file</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.tests.dir</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.out.dir</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.server.host</t>
+  </si>
+  <si>
+    <t>test.nodejs.server.server.port</t>
+  </si>
+  <si>
+    <t>nodejsServerProtoDir</t>
+  </si>
+  <si>
+    <t>nodejsServerLogDir</t>
+  </si>
+  <si>
+    <t>nodejsServerLogFile</t>
+  </si>
+  <si>
+    <t>nodejsServerTestsDir</t>
+  </si>
+  <si>
+    <t>nodejsServerOutDir</t>
+  </si>
+  <si>
+    <t>nodejsServerServerHost</t>
+  </si>
+  <si>
+    <t>nodejsServerServerPort</t>
+  </si>
+  <si>
+    <t>Directory containing .proto files for nodejs server</t>
+  </si>
+  <si>
+    <t>Log directory for NodeJs server</t>
+  </si>
+  <si>
+    <t>Log file for NodeJs server</t>
+  </si>
+  <si>
+    <t>Directory containing NodeJs server .bin test cases</t>
+  </si>
+  <si>
+    <t>Output directory for NodeJs server</t>
+  </si>
+  <si>
+    <t>Hostname of the NodeJs server</t>
+  </si>
+  <si>
+    <t>Port of the NodeJs server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOTE: Server ports inside and outside container should be mapped to the same number </t>
+  </si>
+  <si>
+    <t>node-server.log</t>
+  </si>
+  <si>
+    <t>out/server/</t>
+  </si>
+  <si>
+    <t>NOTE: In Java programs (Core + client/server), directory configs (*.dir) ends without the file separator ("/")</t>
+  </si>
+  <si>
+    <t>test.java.client.tests.dir</t>
+  </si>
+  <si>
+    <t>test.java.client.out.dir</t>
+  </si>
+  <si>
+    <t>test-cases/client</t>
+  </si>
+  <si>
+    <t>out/client</t>
+  </si>
+  <si>
+    <t>tests.dir</t>
+  </si>
+  <si>
+    <t>out.dir</t>
+  </si>
+  <si>
+    <t>javaClientTestsDir</t>
+  </si>
+  <si>
+    <t>javaClientOutDir</t>
+  </si>
+  <si>
+    <t>Test cases directory for Java client</t>
+  </si>
+  <si>
+    <t>Output directory for Java client</t>
+  </si>
+  <si>
+    <t>test.java.client.server.host</t>
+  </si>
+  <si>
+    <t>test.java.client.server.port</t>
+  </si>
+  <si>
+    <t>javaClientServerHost</t>
+  </si>
+  <si>
+    <t>javaClientServerPort</t>
+  </si>
+  <si>
+    <t>Hostname of the server to which Java client connects to</t>
+  </si>
+  <si>
+    <t>Port of the server to which Java client connects to</t>
+  </si>
+  <si>
+    <t>server.host</t>
+  </si>
+  <si>
+    <t>server.port</t>
+  </si>
+  <si>
+    <t>test.java.server.tests.dir</t>
+  </si>
+  <si>
+    <t>test.java.server.out.dir</t>
+  </si>
+  <si>
+    <t>test.java.server.server.port</t>
+  </si>
+  <si>
+    <t>javaServerTestsDir</t>
+  </si>
+  <si>
+    <t>javaServerOutDir</t>
+  </si>
+  <si>
+    <t>javaServerServerPort</t>
+  </si>
+  <si>
+    <t>Test cases directory for Java server</t>
+  </si>
+  <si>
+    <t>Output directory for Java server</t>
+  </si>
+  <si>
+    <t>Port of the Java server</t>
+  </si>
+  <si>
+    <t>test-cases/server</t>
+  </si>
+  <si>
+    <t>out/server</t>
+  </si>
+  <si>
+    <t>NOT_ASSIGNED</t>
+  </si>
+  <si>
+    <t>core.setup.script</t>
+  </si>
+  <si>
+    <t>setup/setup.txt</t>
+  </si>
+  <si>
+    <t>setupScriptFilePath</t>
+  </si>
+  <si>
+    <t>Test setup script (File path)</t>
+  </si>
+  <si>
+    <t>core.test.timeout.ms</t>
+  </si>
+  <si>
+    <t>testTimeoutMillis</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Max waiting time after successfully launch server + client before force quit</t>
+  </si>
+  <si>
+    <t>core.docker.compose.timeout.ms</t>
+  </si>
+  <si>
+    <t>dockerComposeTimeoutMillis</t>
+  </si>
+  <si>
+    <t>Max waiting time for docker compose to build and launch server / client</t>
+  </si>
+  <si>
+    <t>core.cleanup.mode</t>
+  </si>
+  <si>
+    <t>cleanupMode</t>
+  </si>
+  <si>
+    <t>Cleans up temporary files before or after test, or both, or none. Check {@link org.grpctest.core.pojo.CleanupMode} for details</t>
+  </si>
+  <si>
+    <t>CleanupMode</t>
+  </si>
+  <si>
+    <t>core.docker.server.startup.timeout.ms</t>
+  </si>
+  <si>
+    <t>serverStartupTimeoutMillis</t>
+  </si>
+  <si>
+    <t>Max time waiting for server to start (after successful docker compose up server) before launching client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -86,6 +505,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -100,7 +533,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -132,23 +565,114 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -162,16 +686,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:E1048576" totalsRowShown="0">
-  <autoFilter ref="A2:E1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)"/>
-    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="A2:H1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H35">
+    <sortCondition ref="A2:A1048576"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Column4" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="5"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -492,49 +1022,735 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="97.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>132</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" t="s">
+        <v>102</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D19" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" t="s">
+        <v>102</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A3:A1048576">
+    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="test.java.server.">
+      <formula>LEFT(A3,LEN("test.java.server."))="test.java.server."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="test.java.client.">
+      <formula>LEFT(A3,LEN("test.java.client."))="test.java.client."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="2" priority="4" operator="beginsWith" text="test.nodejs.server.">
+      <formula>LEFT(A3,LEN("test.nodejs.server."))="test.nodejs.server."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="1" priority="5" operator="beginsWith" text="test.nodejs.client.">
+      <formula>LEFT(A3,LEN("test.nodejs.client."))="test.nodejs.client."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="0" priority="6" operator="beginsWith" text="core.">
+      <formula>LEFT(A3,LEN("core."))="core."</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C82824-7B5E-8646-8E7C-440799F738D0}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
-    <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Python: Add base + streaming (UNTESTED)
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBFD4A9C-199F-8F4D-BD0A-F3DE1AB7E518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3284354C-06EB-D742-9059-BF497FB3ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" activeTab="1" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="184">
   <si>
     <t>List of all config items</t>
   </si>
@@ -58,9 +57,6 @@
     <t>Name (full config name)</t>
   </si>
   <si>
-    <t>Column4</t>
-  </si>
-  <si>
     <t>Name (Config property)</t>
   </si>
   <si>
@@ -476,6 +472,123 @@
   </si>
   <si>
     <t>Max time waiting for server to start (after successful docker compose up server) before launching client</t>
+  </si>
+  <si>
+    <t>test.python.server.log.dir</t>
+  </si>
+  <si>
+    <t>test.python.server.log.file</t>
+  </si>
+  <si>
+    <t>pyServerLogDir</t>
+  </si>
+  <si>
+    <t>pyServerLogFile</t>
+  </si>
+  <si>
+    <t>Log directory for Python server</t>
+  </si>
+  <si>
+    <t>Log file prefix for Python server</t>
+  </si>
+  <si>
+    <t>Python deploy.yml property</t>
+  </si>
+  <si>
+    <t>log.dir</t>
+  </si>
+  <si>
+    <t>py-server</t>
+  </si>
+  <si>
+    <t>test.python.client.log.dir</t>
+  </si>
+  <si>
+    <t>test.python.client.log.file</t>
+  </si>
+  <si>
+    <t>pyClientLogDir</t>
+  </si>
+  <si>
+    <t>pyClientLogFile</t>
+  </si>
+  <si>
+    <t>Log directory for Python client</t>
+  </si>
+  <si>
+    <t>Log file prefix for Python client</t>
+  </si>
+  <si>
+    <t>py-client</t>
+  </si>
+  <si>
+    <t>test.python.server.out.dir</t>
+  </si>
+  <si>
+    <t>test.python.server.server.port</t>
+  </si>
+  <si>
+    <t>test.python.server.tests.dir</t>
+  </si>
+  <si>
+    <t>in.dir</t>
+  </si>
+  <si>
+    <t>test.python.client.out.dir</t>
+  </si>
+  <si>
+    <t>test.python.client.server.port</t>
+  </si>
+  <si>
+    <t>test.python.client.tests.dir</t>
+  </si>
+  <si>
+    <t>pyServerOutDir</t>
+  </si>
+  <si>
+    <t>pyServerServerPort</t>
+  </si>
+  <si>
+    <t>pyServerTestsDir</t>
+  </si>
+  <si>
+    <t>pyClientOutDir</t>
+  </si>
+  <si>
+    <t>pyClientServerPort</t>
+  </si>
+  <si>
+    <t>pyClientTestsDir</t>
+  </si>
+  <si>
+    <t>Output directory for Python server</t>
+  </si>
+  <si>
+    <t>Port of the Python server</t>
+  </si>
+  <si>
+    <t>Directory containing Python server .bin test cases</t>
+  </si>
+  <si>
+    <t>Output directory for Python client</t>
+  </si>
+  <si>
+    <t>Directory containing Python client .bin test cases</t>
+  </si>
+  <si>
+    <t>log.file_prefix</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>test.python.client.server.host</t>
+  </si>
+  <si>
+    <t>pyClientServerHost</t>
+  </si>
+  <si>
+    <t>Hostname of the server to which Python client connects to</t>
   </si>
 </sst>
 </file>
@@ -594,7 +707,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
     <dxf>
       <fill>
         <patternFill>
@@ -643,6 +756,70 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFAC8E68"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFF672"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -674,6 +851,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFAC8E68"/>
+      <color rgb="FFFFD60A"/>
+      <color rgb="FF929906"/>
+      <color rgb="FFAEB601"/>
+      <color rgb="FF807B18"/>
+      <color rgb="FFFFF672"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -686,20 +873,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A2:H1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H35">
     <sortCondition ref="A2:A1048576"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Column4" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Python deploy.yml property" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1022,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A30" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1035,7 +1222,7 @@
     <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1050,19 +1237,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>151</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -1076,76 +1263,76 @@
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>140</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G3" t="s">
         <v>141</v>
-      </c>
-      <c r="G3" t="s">
-        <v>142</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" t="s">
         <v>136</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>137</v>
       </c>
-      <c r="C6" t="s">
-        <v>138</v>
-      </c>
       <c r="G6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H6">
         <v>300000</v>
@@ -1153,16 +1340,16 @@
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
         <v>143</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>144</v>
       </c>
-      <c r="C7" t="s">
-        <v>145</v>
-      </c>
       <c r="G7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H7">
         <v>300000</v>
@@ -1170,101 +1357,101 @@
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
       <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
         <v>13</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
         <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
         <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
         <v>128</v>
-      </c>
-      <c r="B12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" t="s">
-        <v>131</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" t="s">
         <v>132</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" t="s">
         <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>135</v>
-      </c>
-      <c r="G13" t="s">
-        <v>134</v>
       </c>
       <c r="H13">
         <v>300000</v>
@@ -1272,56 +1459,56 @@
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H16">
         <v>50051</v>
@@ -1329,59 +1516,59 @@
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19">
         <v>50051</v>
@@ -1389,136 +1576,136 @@
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
         <v>43</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" t="s">
         <v>44</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
       <c r="E23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
         <v>55</v>
-      </c>
-      <c r="G23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
         <v>70</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
       <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" t="s">
         <v>35</v>
-      </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
         <v>63</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>64</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>65</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>66</v>
-      </c>
-      <c r="G26" t="s">
-        <v>67</v>
       </c>
       <c r="H26">
         <v>50051</v>
@@ -1526,139 +1713,139 @@
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
         <v>47</v>
       </c>
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" t="s">
         <v>48</v>
-      </c>
-      <c r="G27" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
         <v>35</v>
-      </c>
-      <c r="G31" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" t="s">
         <v>66</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
       </c>
       <c r="H33">
         <v>50051</v>
@@ -1666,41 +1853,264 @@
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" t="s">
         <v>48</v>
       </c>
-      <c r="G34" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" t="s">
-        <v>49</v>
+    </row>
+    <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" t="s">
+        <v>152</v>
+      </c>
+      <c r="G35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>146</v>
+      </c>
+      <c r="B36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" t="s">
+        <v>150</v>
+      </c>
+      <c r="F36" t="s">
+        <v>179</v>
+      </c>
+      <c r="G36" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F37" t="s">
+        <v>152</v>
+      </c>
+      <c r="G37" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>155</v>
+      </c>
+      <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" t="s">
+        <v>179</v>
+      </c>
+      <c r="G38" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>161</v>
+      </c>
+      <c r="B39" t="s">
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" t="s">
+        <v>102</v>
+      </c>
+      <c r="G39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>162</v>
+      </c>
+      <c r="B40" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" t="s">
+        <v>175</v>
+      </c>
+      <c r="F40" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>163</v>
+      </c>
+      <c r="B41" t="s">
+        <v>170</v>
+      </c>
+      <c r="C41" t="s">
+        <v>176</v>
+      </c>
+      <c r="F41" t="s">
+        <v>164</v>
+      </c>
+      <c r="G41" t="s">
+        <v>12</v>
+      </c>
+      <c r="H41" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" t="s">
+        <v>177</v>
+      </c>
+      <c r="F42" t="s">
+        <v>102</v>
+      </c>
+      <c r="G42" t="s">
+        <v>12</v>
+      </c>
+      <c r="H42" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G43" t="s">
+        <v>66</v>
+      </c>
+      <c r="H43">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="test.java.server.">
+    <cfRule type="beginsWith" dxfId="6" priority="4" operator="beginsWith" text="test.java.server.">
       <formula>LEFT(A3,LEN("test.java.server."))="test.java.server."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="3" operator="beginsWith" text="test.java.client.">
+    <cfRule type="beginsWith" dxfId="7" priority="5" operator="beginsWith" text="test.java.client.">
       <formula>LEFT(A3,LEN("test.java.client."))="test.java.client."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="2" priority="4" operator="beginsWith" text="test.nodejs.server.">
+    <cfRule type="beginsWith" dxfId="8" priority="6" operator="beginsWith" text="test.nodejs.server.">
       <formula>LEFT(A3,LEN("test.nodejs.server."))="test.nodejs.server."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="5" operator="beginsWith" text="test.nodejs.client.">
+    <cfRule type="beginsWith" dxfId="9" priority="7" operator="beginsWith" text="test.nodejs.client.">
       <formula>LEFT(A3,LEN("test.nodejs.client."))="test.nodejs.client."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="0" priority="6" operator="beginsWith" text="core.">
+    <cfRule type="beginsWith" dxfId="10" priority="8" operator="beginsWith" text="core.">
       <formula>LEFT(A3,LEN("core."))="core."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="11" priority="2" operator="beginsWith" text="test.python.client">
+      <formula>LEFT(A3,LEN("test.python.client"))="test.python.client"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="1" operator="beginsWith" text="test.python.server">
+      <formula>LEFT(A3,LEN("test.python.server"))="test.python.server"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1713,10 +2123,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C82824-7B5E-8646-8E7C-440799F738D0}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1726,28 +2136,33 @@
   <sheetData>
     <row r="1" spans="1:1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basic data type test + fixed python and nodejs bugs
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3284354C-06EB-D742-9059-BF497FB3ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A41810B-0D3F-7A43-8117-2E4670B761A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" activeTab="1" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="185">
   <si>
     <t>List of all config items</t>
   </si>
@@ -589,6 +590,9 @@
   </si>
   <si>
     <t>Hostname of the server to which Python client connects to</t>
+  </si>
+  <si>
+    <t>Port of the server to which Python client connects to</t>
   </si>
 </sst>
 </file>
@@ -707,7 +711,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -756,12 +760,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFAC8E68"/>
+          <bgColor rgb="FFFFF672"/>
         </patternFill>
       </fill>
     </dxf>
@@ -771,51 +772,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFF672"/>
+          <bgColor rgb="FFAC8E68"/>
         </patternFill>
       </fill>
     </dxf>
@@ -873,20 +830,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A2:H1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H46">
     <sortCondition ref="A2:A1048576"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Python deploy.yml property" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Python deploy.yml property" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1211,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1873,13 +1830,13 @@
     </row>
     <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B35" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="C35" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="F35" t="s">
         <v>152</v>
@@ -1893,13 +1850,13 @@
     </row>
     <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C36" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="F36" t="s">
         <v>179</v>
@@ -1908,209 +1865,209 @@
         <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B37" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="F37" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C38" t="s">
-        <v>159</v>
+        <v>183</v>
       </c>
       <c r="F38" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>
-      </c>
-      <c r="H38" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="B39" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C39" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
-        <v>125</v>
+        <v>66</v>
+      </c>
+      <c r="H39">
+        <v>50051</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C40" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F40" t="s">
-        <v>114</v>
+        <v>164</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
-      </c>
-      <c r="H40">
-        <v>50051</v>
+        <v>12</v>
+      </c>
+      <c r="H40" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="F41" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="G41" t="s">
         <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="F42" t="s">
-        <v>102</v>
+        <v>179</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>100</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B43" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F43" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>66</v>
-      </c>
-      <c r="H43">
-        <v>50051</v>
+        <v>12</v>
+      </c>
+      <c r="H43" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B44" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F44" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
-      </c>
-      <c r="H44" t="s">
-        <v>99</v>
+        <v>66</v>
+      </c>
+      <c r="H44">
+        <v>50051</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="F45" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="G45" t="s">
         <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A3:A1048576">
-    <cfRule type="beginsWith" dxfId="6" priority="4" operator="beginsWith" text="test.java.server.">
+    <cfRule type="beginsWith" dxfId="6" priority="1" operator="beginsWith" text="test.python.server">
+      <formula>LEFT(A3,LEN("test.python.server"))="test.python.server"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="5" priority="2" operator="beginsWith" text="test.python.client">
+      <formula>LEFT(A3,LEN("test.python.client"))="test.python.client"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="test.java.server.">
       <formula>LEFT(A3,LEN("test.java.server."))="test.java.server."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="5" operator="beginsWith" text="test.java.client.">
+    <cfRule type="beginsWith" dxfId="3" priority="5" operator="beginsWith" text="test.java.client.">
       <formula>LEFT(A3,LEN("test.java.client."))="test.java.client."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="6" operator="beginsWith" text="test.nodejs.server.">
+    <cfRule type="beginsWith" dxfId="2" priority="6" operator="beginsWith" text="test.nodejs.server.">
       <formula>LEFT(A3,LEN("test.nodejs.server."))="test.nodejs.server."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="9" priority="7" operator="beginsWith" text="test.nodejs.client.">
+    <cfRule type="beginsWith" dxfId="1" priority="7" operator="beginsWith" text="test.nodejs.client.">
       <formula>LEFT(A3,LEN("test.nodejs.client."))="test.nodejs.client."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="8" operator="beginsWith" text="core.">
+    <cfRule type="beginsWith" dxfId="0" priority="8" operator="beginsWith" text="core.">
       <formula>LEFT(A3,LEN("core."))="core."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="11" priority="2" operator="beginsWith" text="test.python.client">
-      <formula>LEFT(A3,LEN("test.python.client"))="test.python.client"</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="1" operator="beginsWith" text="test.python.server">
-      <formula>LEFT(A3,LEN("test.python.server"))="test.python.server"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2125,7 +2082,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C82824-7B5E-8646-8E7C-440799F738D0}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix bugs during test, update test progress (finished basic data types test), add field logging (UNTESTED)
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4A41810B-0D3F-7A43-8117-2E4670B761A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{31403A25-A0F2-D143-9DAB-D5DFB2EB9EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="209">
   <si>
     <t>List of all config items</t>
   </si>
@@ -593,6 +593,78 @@
   </si>
   <si>
     <t>Port of the server to which Python client connects to</t>
+  </si>
+  <si>
+    <t>core.test.client.log.request</t>
+  </si>
+  <si>
+    <t>clientLogRequests</t>
+  </si>
+  <si>
+    <t>Log requests to be sent from the client (in the client log)</t>
+  </si>
+  <si>
+    <t>clientLogRequestsPrintFields</t>
+  </si>
+  <si>
+    <t>Log each fields of the requests to be sent from the client (in the client log)</t>
+  </si>
+  <si>
+    <t>core.test.client.log.response</t>
+  </si>
+  <si>
+    <t>core.test.client.log.response.print-fields</t>
+  </si>
+  <si>
+    <t>core.test.client.log.request.print-fields</t>
+  </si>
+  <si>
+    <t>clientLogResponses</t>
+  </si>
+  <si>
+    <t>clientLogResponsesPrintFields</t>
+  </si>
+  <si>
+    <t>Log responses received by the client (in the client log)</t>
+  </si>
+  <si>
+    <t>Log each fields of the responses received by the client (in the client log)</t>
+  </si>
+  <si>
+    <t>core.test.server.log.request</t>
+  </si>
+  <si>
+    <t>core.test.server.log.request.print-fields</t>
+  </si>
+  <si>
+    <t>serverLogRequests</t>
+  </si>
+  <si>
+    <t>serverLogRequestsPrintFields</t>
+  </si>
+  <si>
+    <t>Log each fields of the requests received by the server(in the server log)</t>
+  </si>
+  <si>
+    <t>Log requests received by the server (in the server log)</t>
+  </si>
+  <si>
+    <t>core.test.server.log.response</t>
+  </si>
+  <si>
+    <t>core.test.server.log.response.print-fields</t>
+  </si>
+  <si>
+    <t>serverLogResponsesPrintFields</t>
+  </si>
+  <si>
+    <t>serverLogResponses</t>
+  </si>
+  <si>
+    <t>Log responses to be sent from the server (in the server log)</t>
+  </si>
+  <si>
+    <t>Log each fields of the responses to be sent from the server (in the server log)</t>
   </si>
 </sst>
 </file>
@@ -832,7 +904,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A2:H1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H46">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H54">
     <sortCondition ref="A2:A1048576"/>
   </sortState>
   <tableColumns count="8">
@@ -1166,16 +1238,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -1399,649 +1471,785 @@
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>187</v>
       </c>
       <c r="G13" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13">
-        <v>300000</v>
+        <v>33</v>
+      </c>
+      <c r="H13" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>98</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>188</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D14" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>100</v>
+        <v>33</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>190</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="H15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>108</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>114</v>
+        <v>196</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16">
-        <v>50051</v>
+        <v>33</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>197</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>199</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
-        <v>99</v>
+        <v>33</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>198</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D18" t="s">
-        <v>102</v>
+        <v>201</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" t="s">
-        <v>125</v>
+        <v>33</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>206</v>
       </c>
       <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19">
-        <v>50051</v>
+        <v>33</v>
+      </c>
+      <c r="H19" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>204</v>
       </c>
       <c r="B20" t="s">
-        <v>118</v>
+        <v>205</v>
       </c>
       <c r="C20" t="s">
-        <v>121</v>
-      </c>
-      <c r="D20" t="s">
-        <v>101</v>
+        <v>208</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" t="s">
-        <v>124</v>
+        <v>33</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>131</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>132</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>36</v>
+        <v>134</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>38</v>
+        <v>133</v>
+      </c>
+      <c r="H21">
+        <v>300000</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>104</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>37</v>
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>102</v>
       </c>
       <c r="G22" t="s">
         <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" t="s">
-        <v>54</v>
+        <v>111</v>
+      </c>
+      <c r="D23" t="s">
+        <v>113</v>
       </c>
       <c r="G23" t="s">
         <v>12</v>
-      </c>
-      <c r="H23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" t="s">
-        <v>34</v>
+        <v>112</v>
+      </c>
+      <c r="D24" t="s">
+        <v>114</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" t="s">
-        <v>35</v>
+        <v>66</v>
+      </c>
+      <c r="H24">
+        <v>50051</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>59</v>
+        <v>105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>101</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>119</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
+        <v>122</v>
+      </c>
+      <c r="D26" t="s">
+        <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26">
-        <v>50051</v>
+        <v>12</v>
+      </c>
+      <c r="H26" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E27" t="s">
-        <v>47</v>
+        <v>123</v>
+      </c>
+      <c r="D27" t="s">
+        <v>114</v>
       </c>
       <c r="G27" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" t="s">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="H27">
+        <v>50051</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" t="s">
-        <v>36</v>
+        <v>121</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
       </c>
       <c r="G28" t="s">
         <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>38</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G29" t="s">
         <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="E30" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="G30" t="s">
         <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="G31" t="s">
         <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E32" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="G32" t="s">
         <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="B33" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G33" t="s">
-        <v>66</v>
-      </c>
-      <c r="H33">
-        <v>50051</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="E34" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G34" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" t="s">
-        <v>48</v>
+        <v>66</v>
+      </c>
+      <c r="H34">
+        <v>50051</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>158</v>
-      </c>
-      <c r="F35" t="s">
-        <v>152</v>
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>47</v>
       </c>
       <c r="G35" t="s">
         <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>180</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="C36" t="s">
-        <v>159</v>
-      </c>
-      <c r="F36" t="s">
-        <v>179</v>
+        <v>87</v>
+      </c>
+      <c r="E36" t="s">
+        <v>36</v>
       </c>
       <c r="G36" t="s">
         <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>165</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>171</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
-      </c>
-      <c r="F37" t="s">
-        <v>102</v>
+        <v>88</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
       </c>
       <c r="G37" t="s">
         <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>182</v>
+        <v>83</v>
       </c>
       <c r="C38" t="s">
-        <v>183</v>
-      </c>
-      <c r="F38" t="s">
-        <v>113</v>
+        <v>90</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
       </c>
       <c r="G38" t="s">
         <v>12</v>
+      </c>
+      <c r="H38" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>79</v>
       </c>
       <c r="C39" t="s">
-        <v>184</v>
-      </c>
-      <c r="F39" t="s">
-        <v>114</v>
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
+        <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>66</v>
-      </c>
-      <c r="H39">
-        <v>50051</v>
+        <v>12</v>
+      </c>
+      <c r="H39" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>167</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>173</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>178</v>
-      </c>
-      <c r="F40" t="s">
-        <v>164</v>
+        <v>91</v>
+      </c>
+      <c r="E40" t="s">
+        <v>59</v>
       </c>
       <c r="G40" t="s">
         <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>145</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>149</v>
-      </c>
-      <c r="F41" t="s">
-        <v>152</v>
+        <v>92</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
       </c>
       <c r="G41" t="s">
-        <v>12</v>
-      </c>
-      <c r="H41" t="s">
-        <v>180</v>
+        <v>66</v>
+      </c>
+      <c r="H41">
+        <v>50051</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>148</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>150</v>
-      </c>
-      <c r="F42" t="s">
-        <v>179</v>
+        <v>89</v>
+      </c>
+      <c r="E42" t="s">
+        <v>47</v>
       </c>
       <c r="G42" t="s">
         <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C43" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="F43" t="s">
-        <v>102</v>
+        <v>152</v>
       </c>
       <c r="G43" t="s">
         <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>125</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C44" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="F44" t="s">
-        <v>114</v>
+        <v>179</v>
       </c>
       <c r="G44" t="s">
-        <v>66</v>
-      </c>
-      <c r="H44">
-        <v>50051</v>
+        <v>12</v>
+      </c>
+      <c r="H44" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" t="s">
+        <v>171</v>
+      </c>
+      <c r="C45" t="s">
+        <v>177</v>
+      </c>
+      <c r="F45" t="s">
+        <v>102</v>
+      </c>
+      <c r="G45" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" t="s">
+        <v>182</v>
+      </c>
+      <c r="C46" t="s">
+        <v>183</v>
+      </c>
+      <c r="F46" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" t="s">
+        <v>184</v>
+      </c>
+      <c r="F47" t="s">
+        <v>114</v>
+      </c>
+      <c r="G47" t="s">
+        <v>66</v>
+      </c>
+      <c r="H47">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>167</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+      <c r="F48" t="s">
+        <v>164</v>
+      </c>
+      <c r="G48" t="s">
+        <v>12</v>
+      </c>
+      <c r="H48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>145</v>
+      </c>
+      <c r="B49" t="s">
+        <v>147</v>
+      </c>
+      <c r="C49" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" t="s">
+        <v>152</v>
+      </c>
+      <c r="G49" t="s">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" t="s">
+        <v>148</v>
+      </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
+      <c r="F50" t="s">
+        <v>179</v>
+      </c>
+      <c r="G50" t="s">
+        <v>12</v>
+      </c>
+      <c r="H50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" t="s">
+        <v>174</v>
+      </c>
+      <c r="F51" t="s">
+        <v>102</v>
+      </c>
+      <c r="G51" t="s">
+        <v>12</v>
+      </c>
+      <c r="H51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" t="s">
+        <v>175</v>
+      </c>
+      <c r="F52" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" t="s">
+        <v>66</v>
+      </c>
+      <c r="H52">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>163</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B53" t="s">
         <v>170</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C53" t="s">
         <v>176</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F53" t="s">
         <v>164</v>
       </c>
-      <c r="G45" t="s">
-        <v>12</v>
-      </c>
-      <c r="H45" t="s">
+      <c r="G53" t="s">
+        <v>12</v>
+      </c>
+      <c r="H53" t="s">
         <v>124</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added map testing and bug fixes
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31403A25-A0F2-D143-9DAB-D5DFB2EB9EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E98866E2-9B5A-BD41-BB0D-23E63EFE0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" activeTab="1" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CONFIGS" sheetId="1" r:id="rId1"/>
+    <sheet name="CONSTANTS" sheetId="3" r:id="rId2"/>
+    <sheet name="ENUMS" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="217">
   <si>
     <t>List of all config items</t>
   </si>
@@ -67,69 +68,24 @@
     <t>Java application.properties property</t>
   </si>
   <si>
-    <t>core.log.dir</t>
-  </si>
-  <si>
-    <t>logDir</t>
-  </si>
-  <si>
-    <t>Log directory for CoreService</t>
-  </si>
-  <si>
     <t>String</t>
   </si>
   <si>
     <t>./log</t>
   </si>
   <si>
-    <t>core.proto.descriptor.path</t>
-  </si>
-  <si>
-    <t>protoDescriptorPath</t>
-  </si>
-  <si>
-    <t>Path to .protobin file</t>
-  </si>
-  <si>
     <t>protobin/common.protobin</t>
   </si>
   <si>
-    <t>core.custom-tests.classpath</t>
-  </si>
-  <si>
-    <t>customTestsClasspath</t>
-  </si>
-  <si>
     <t>tests</t>
   </si>
   <si>
-    <t>core.proto.classpath</t>
-  </si>
-  <si>
-    <t>protoClasspath</t>
-  </si>
-  <si>
-    <t>Classpath to directory containing .proto files</t>
-  </si>
-  <si>
     <t>proto</t>
   </si>
   <si>
-    <t>Classpath to directory containing test cases (CoreService will translate these test cases to .bin files in test-cases/)</t>
-  </si>
-  <si>
-    <t>testsDir</t>
-  </si>
-  <si>
     <t>Directory containing .bin test cases</t>
   </si>
   <si>
-    <t>core.out.tests.dir</t>
-  </si>
-  <si>
-    <t>test-cases</t>
-  </si>
-  <si>
     <t>core.dev.debug.enabled</t>
   </si>
   <si>
@@ -220,9 +176,6 @@
     <t>config.server.host</t>
   </si>
   <si>
-    <t>APPENDIX A: LIST OF CONSTANTS</t>
-  </si>
-  <si>
     <t>SERVER HOSTNAME</t>
   </si>
   <si>
@@ -665,6 +618,78 @@
   </si>
   <si>
     <t>Log each fields of the responses to be sent from the server (in the server log)</t>
+  </si>
+  <si>
+    <t>Directory containing .bin test cases (for client)</t>
+  </si>
+  <si>
+    <t>Directory containing .bin test cases (for server)</t>
+  </si>
+  <si>
+    <t>Output directory of server</t>
+  </si>
+  <si>
+    <t>Output directory of client</t>
+  </si>
+  <si>
+    <t>LIST OF USEFUL ENUMS FOR USERS</t>
+  </si>
+  <si>
+    <t>Note: Enums here are "variables which can only be assigned to one of the listed values". They are not necessarily be defined as enum in source code. This is for user reference.</t>
+  </si>
+  <si>
+    <t>LIST OF CONSTANTS</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>TEST_PROGRAM_MAX_WAIT_TIMEOUT_MS</t>
+  </si>
+  <si>
+    <t>TEST_PROGRAM_DEFAULT_POLL_INTERVAL_MS</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>CUSTOM_TESTS_CLASSPATH</t>
+  </si>
+  <si>
+    <t>Custom test case location</t>
+  </si>
+  <si>
+    <t>LOG_DIR</t>
+  </si>
+  <si>
+    <t>Log directory (core service)</t>
+  </si>
+  <si>
+    <t>OUT_DIR_CLIENT</t>
+  </si>
+  <si>
+    <t>OUT_DIR_SERVER</t>
+  </si>
+  <si>
+    <t>PROTO_CLASSPATH</t>
+  </si>
+  <si>
+    <t>Proto file location</t>
+  </si>
+  <si>
+    <t>PROTO_DESCRIPTOR_PATH'</t>
+  </si>
+  <si>
+    <t>Proto descriptor file</t>
+  </si>
+  <si>
+    <t>TESTS_DIR_CLIENT</t>
+  </si>
+  <si>
+    <t>TESTS_DIR_SERVER</t>
   </si>
 </sst>
 </file>
@@ -783,7 +808,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -849,6 +874,13 @@
       </fill>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color theme="4" tint="0.499984740745262"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -902,22 +934,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048576" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A2:H1048576" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H54">
-    <sortCondition ref="A2:A1048576"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048575" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A2:H1048575" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H57">
+    <sortCondition ref="A2:A1048575"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Python deploy.yml property" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{0D341317-1B7E-6C49-81BD-5096283C100A}" name="Name (full config name)" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{92CB9853-6A84-C54E-950A-83FAFBC10635}" name="Name (Config property)" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{77F1508D-9BE8-D044-A2D4-3B197FF73157}" name="Description" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{55E322F5-BA4B-794E-9F7C-CE7E425D58F2}" name="Java application.properties property" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{A81EE9CF-7AE5-AE4F-AAFE-FD04266102B8}" name="NodeJS deploy.js property" dataDxfId="11"/>
+    <tableColumn id="8" xr3:uid="{E2C513DB-F477-E941-86F8-7E02995B3AFB}" name="Python deploy.yml property" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{FF77A0A4-6934-F44E-A9A4-EB82FE3CEF64}" name="Type" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{F0DAB00A-2F6A-B447-800F-FE9ACCA786C5}" name="Default value" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{867D151E-5813-DB40-8EC7-978D12769742}" name="Table3" displayName="Table3" ref="A3:D13" totalsRowShown="0">
+  <autoFilter ref="A3:D13" xr:uid="{867D151E-5813-DB40-8EC7-978D12769742}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{88EC302F-8F85-CF43-8FD5-AEA29CC6EFA7}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{89D9426D-C8AD-E246-937B-8C1E0AE9F757}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{2BCF2E7B-6015-8C4E-B933-C762D1DE46D5}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{465CDBAB-D969-5345-9C26-569AB5D30ECC}" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF795C9D-9ECD-5F40-8CA6-AC7A9EB63075}" name="Table2" displayName="Table2" ref="A3:A7" totalsRowShown="0" headerRowBorderDxfId="7" headerRowCellStyle="Heading 2">
+  <autoFilter ref="A3:A7" xr:uid="{EF795C9D-9ECD-5F40-8CA6-AC7A9EB63075}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B7E3F614-A665-8742-8B96-9ABA5729F4A9}" name="SERVER HOSTNAME"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1238,10 +1293,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1278,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
@@ -1292,195 +1347,110 @@
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
+      <c r="H4" t="b">
+        <v>0</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>121</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
+        <v>117</v>
+      </c>
+      <c r="H5">
+        <v>300000</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G6" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>142</v>
-      </c>
-      <c r="B7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H11" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
-        <v>129</v>
+        <v>170</v>
       </c>
       <c r="C12" t="s">
-        <v>130</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>128</v>
+        <v>18</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B13" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="C13" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
@@ -1488,16 +1458,16 @@
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B14" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
@@ -1505,16 +1475,16 @@
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="C15" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H15" t="b">
         <v>1</v>
@@ -1522,16 +1492,16 @@
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H16" t="b">
         <v>1</v>
@@ -1539,16 +1509,16 @@
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="C17" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H17" t="b">
         <v>1</v>
@@ -1556,16 +1526,16 @@
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B18" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="G18" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H18" t="b">
         <v>1</v>
@@ -1573,16 +1543,16 @@
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B19" t="s">
-        <v>206</v>
+        <v>189</v>
       </c>
       <c r="C19" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="H19" t="b">
         <v>1</v>
@@ -1590,672 +1560,672 @@
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="B20" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="C20" t="s">
-        <v>208</v>
+        <v>118</v>
       </c>
       <c r="G20" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="H20">
+        <v>300000</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C21" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="H21">
         <v>300000</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" t="s">
-        <v>100</v>
-      </c>
-    </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="H23" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="G24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H24">
-        <v>50051</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="H25">
+        <v>50051</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
-      </c>
-      <c r="H27">
-        <v>50051</v>
+        <v>9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C28" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
-        <v>124</v>
+        <v>50</v>
+      </c>
+      <c r="H28">
+        <v>50051</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" t="s">
-        <v>36</v>
+        <v>105</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
       </c>
       <c r="G29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H29" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="G31" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H31" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H32" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="G33" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
-      </c>
-      <c r="H34">
-        <v>50051</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="H35">
+        <v>50051</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G36" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H36" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="E37" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H37" t="s">
-        <v>94</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="G38" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H38" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" t="s">
         <v>79</v>
-      </c>
-      <c r="C39" t="s">
-        <v>86</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="G40" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C41" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="E41" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="G41" t="s">
-        <v>66</v>
-      </c>
-      <c r="H41">
-        <v>50051</v>
+        <v>9</v>
+      </c>
+      <c r="H41" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E42" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G42" t="s">
-        <v>12</v>
-      </c>
-      <c r="H42" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="H42">
+        <v>50051</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="B43" t="s">
-        <v>156</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>158</v>
-      </c>
-      <c r="F43" t="s">
-        <v>152</v>
+        <v>73</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
       </c>
       <c r="G43" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H43" t="s">
-        <v>180</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="B44" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="G44" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H44" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="C45" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="G45" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H45" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="F46" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="G46" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="H46" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" t="s">
         <v>166</v>
       </c>
-      <c r="B47" t="s">
-        <v>172</v>
-      </c>
       <c r="C47" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F47" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="G47" t="s">
-        <v>66</v>
-      </c>
-      <c r="H47">
-        <v>50051</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="B48" t="s">
-        <v>173</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="F48" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="G48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" t="s">
-        <v>99</v>
+        <v>50</v>
+      </c>
+      <c r="H48">
+        <v>50051</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B49" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="F49" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H49" t="s">
-        <v>180</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="F50" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="G50" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H50" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="B51" t="s">
-        <v>168</v>
+        <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="F51" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="G51" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H51" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C52" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="F52" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
       <c r="G52" t="s">
-        <v>66</v>
-      </c>
-      <c r="H52">
-        <v>50051</v>
+        <v>9</v>
+      </c>
+      <c r="H52" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>176</v>
+        <v>159</v>
       </c>
       <c r="F53" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="G53" t="s">
-        <v>12</v>
-      </c>
-      <c r="H53" t="s">
-        <v>124</v>
+        <v>50</v>
+      </c>
+      <c r="H53">
+        <v>50051</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" t="s">
+        <v>154</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" t="s">
+        <v>148</v>
+      </c>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+      <c r="H54" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A3:A1048576">
+  <conditionalFormatting sqref="A3:A1048575">
     <cfRule type="beginsWith" dxfId="6" priority="1" operator="beginsWith" text="test.python.server">
       <formula>LEFT(A3,LEN("test.python.server"))="test.python.server"</formula>
     </cfRule>
@@ -2287,50 +2257,234 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C82824-7B5E-8646-8E7C-440799F738D0}">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE39567F-D25F-5743-8B43-9C604D509CAC}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.5" customWidth="1"/>
+    <col min="2" max="2" width="86.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+      <c r="C4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+      <c r="C5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>207</v>
+      </c>
+      <c r="B7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C82824-7B5E-8646-8E7C-440799F738D0}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:2" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added map testing, fixed bugs
</commit_message>
<xml_diff>
--- a/configs.xlsx
+++ b/configs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Duriana/Documents/Ketchups/FYP/grpc/grpc-auto-test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E98866E2-9B5A-BD41-BB0D-23E63EFE0F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BB6C4A-A1AA-BE48-922A-91FED4BA374C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" activeTab="1" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="24400" windowHeight="14900" xr2:uid="{D0A1C80A-E2F4-3840-9379-6662C4454D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="CONFIGS" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="ENUMS" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -936,7 +935,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}" name="Table1" displayName="Table1" ref="A2:H1048575" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:H1048575" xr:uid="{44741525-A6C2-3143-977F-F35A3B466D2C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H57">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H55">
     <sortCondition ref="A2:A1048575"/>
   </sortState>
   <tableColumns count="8">
@@ -1293,20 +1292,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA5D2EB-AE8E-ED41-A7EB-93349B3876EB}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="91" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="97.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1405,32 +1405,117 @@
         <v>80</v>
       </c>
     </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H6">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" t="s">
+        <v>179</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>180</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" t="s">
-        <v>112</v>
+        <v>18</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="B12" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="C12" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
@@ -1441,13 +1526,13 @@
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="C13" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
@@ -1458,13 +1543,13 @@
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
@@ -1475,13 +1560,13 @@
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
@@ -1492,492 +1577,524 @@
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>183</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>118</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="H16">
+        <v>300000</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>182</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>185</v>
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="H17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>93</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>97</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>188</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>189</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>192</v>
+        <v>96</v>
+      </c>
+      <c r="D19" t="s">
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>50051</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>116</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>85</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
-      </c>
-      <c r="H20">
-        <v>300000</v>
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>128</v>
+        <v>106</v>
+      </c>
+      <c r="D21" t="s">
+        <v>86</v>
       </c>
       <c r="G21" t="s">
-        <v>117</v>
-      </c>
-      <c r="H21">
-        <v>300000</v>
+        <v>9</v>
+      </c>
+      <c r="H21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>50051</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>84</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" t="s">
-        <v>97</v>
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
       </c>
       <c r="G24" t="s">
         <v>9</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" t="s">
-        <v>98</v>
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
       </c>
       <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25">
-        <v>50051</v>
+        <v>9</v>
+      </c>
+      <c r="H25" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" t="s">
-        <v>85</v>
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>39</v>
       </c>
       <c r="G26" t="s">
         <v>9</v>
       </c>
       <c r="H26" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" t="s">
-        <v>86</v>
+        <v>55</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
       </c>
       <c r="G27" t="s">
         <v>9</v>
       </c>
       <c r="H27" t="s">
-        <v>109</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>101</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" t="s">
-        <v>98</v>
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
       </c>
       <c r="G28" t="s">
-        <v>50</v>
-      </c>
-      <c r="H28">
-        <v>50051</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" t="s">
-        <v>85</v>
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" t="s">
-        <v>108</v>
+        <v>50</v>
+      </c>
+      <c r="H29">
+        <v>50051</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G30" t="s">
         <v>9</v>
       </c>
       <c r="H30" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31" t="s">
         <v>9</v>
       </c>
       <c r="H31" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="G32" t="s">
         <v>9</v>
       </c>
       <c r="H32" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="G33" t="s">
         <v>9</v>
       </c>
       <c r="H33" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="G34" t="s">
         <v>9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s">
-        <v>50</v>
-      </c>
-      <c r="H35">
-        <v>50051</v>
+        <v>9</v>
+      </c>
+      <c r="H35" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="G36" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" t="s">
-        <v>33</v>
+        <v>50</v>
+      </c>
+      <c r="H36">
+        <v>50051</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G37" t="s">
         <v>9</v>
       </c>
       <c r="H37" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38" t="s">
-        <v>22</v>
+        <v>142</v>
+      </c>
+      <c r="F38" t="s">
+        <v>136</v>
       </c>
       <c r="G38" t="s">
         <v>9</v>
       </c>
       <c r="H38" t="s">
-        <v>78</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E39" t="s">
-        <v>39</v>
+        <v>143</v>
+      </c>
+      <c r="F39" t="s">
+        <v>163</v>
       </c>
       <c r="G39" t="s">
         <v>9</v>
       </c>
       <c r="H39" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
+        <v>161</v>
+      </c>
+      <c r="F40" t="s">
+        <v>86</v>
       </c>
       <c r="G40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>165</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
-      </c>
-      <c r="E41" t="s">
-        <v>44</v>
+        <v>167</v>
+      </c>
+      <c r="F41" t="s">
+        <v>97</v>
       </c>
       <c r="G41" t="s">
         <v>9</v>
-      </c>
-      <c r="H41" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>150</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E42" t="s">
-        <v>49</v>
+        <v>168</v>
+      </c>
+      <c r="F42" t="s">
+        <v>98</v>
       </c>
       <c r="G42" t="s">
         <v>50</v>
@@ -1988,33 +2105,33 @@
     </row>
     <row r="43" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>151</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="C43" t="s">
-        <v>73</v>
-      </c>
-      <c r="E43" t="s">
-        <v>32</v>
+        <v>162</v>
+      </c>
+      <c r="F43" t="s">
+        <v>148</v>
       </c>
       <c r="G43" t="s">
         <v>9</v>
       </c>
       <c r="H43" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B44" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C44" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
         <v>136</v>
@@ -2028,13 +2145,13 @@
     </row>
     <row r="45" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B45" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C45" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F45" t="s">
         <v>163</v>
@@ -2043,18 +2160,18 @@
         <v>9</v>
       </c>
       <c r="H45" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F46" t="s">
         <v>86</v>
@@ -2063,163 +2180,46 @@
         <v>9</v>
       </c>
       <c r="H46" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F47" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G47" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="H47">
+        <v>50051</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F48" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="G48" t="s">
-        <v>50</v>
-      </c>
-      <c r="H48">
-        <v>50051</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>151</v>
-      </c>
-      <c r="B49" t="s">
-        <v>157</v>
-      </c>
-      <c r="C49" t="s">
-        <v>162</v>
-      </c>
-      <c r="F49" t="s">
-        <v>148</v>
-      </c>
-      <c r="G49" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" t="s">
-        <v>131</v>
-      </c>
-      <c r="C50" t="s">
-        <v>133</v>
-      </c>
-      <c r="F50" t="s">
-        <v>136</v>
-      </c>
-      <c r="G50" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>130</v>
-      </c>
-      <c r="B51" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" t="s">
-        <v>134</v>
-      </c>
-      <c r="F51" t="s">
-        <v>163</v>
-      </c>
-      <c r="G51" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>145</v>
-      </c>
-      <c r="B52" t="s">
-        <v>152</v>
-      </c>
-      <c r="C52" t="s">
-        <v>158</v>
-      </c>
-      <c r="F52" t="s">
-        <v>86</v>
-      </c>
-      <c r="G52" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>146</v>
-      </c>
-      <c r="B53" t="s">
-        <v>153</v>
-      </c>
-      <c r="C53" t="s">
-        <v>159</v>
-      </c>
-      <c r="F53" t="s">
-        <v>98</v>
-      </c>
-      <c r="G53" t="s">
-        <v>50</v>
-      </c>
-      <c r="H53">
-        <v>50051</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>147</v>
-      </c>
-      <c r="B54" t="s">
-        <v>154</v>
-      </c>
-      <c r="C54" t="s">
-        <v>160</v>
-      </c>
-      <c r="F54" t="s">
-        <v>148</v>
-      </c>
-      <c r="G54" t="s">
-        <v>9</v>
-      </c>
-      <c r="H54" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE39567F-D25F-5743-8B43-9C604D509CAC}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>

</xml_diff>